<commit_message>
Update demo list 1
</commit_message>
<xml_diff>
--- a/demos.xlsx
+++ b/demos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsui/Documents/GitHub/atsuihk.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53D71B8C-527F-5749-9F17-94012C18D3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB59AEF-7408-3C42-B460-4FE089E57DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16080" xr2:uid="{78869667-DC14-C34D-8E40-751570D61855}"/>
+    <workbookView xWindow="1160" yWindow="940" windowWidth="28240" windowHeight="16080" xr2:uid="{78869667-DC14-C34D-8E40-751570D61855}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Picture</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,11 +50,86 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQFfUnCIPVTtIm4RpwIrOehAhXxNXeuKY2TZQ&amp;s</t>
+    <t>Extract the built area from Sentinel 2 satellite images, intersect the area with the new towns, and create 100m buffer by cycle tracks. Calculate the percentage of buffer to the built area of each new town in HK.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unmarried Males to Females ratio with C&amp;SD 2021 Population Census, Hong Kong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://arcg.is/v4Oq4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.arcgis.com/apps/dashboards/f3749165d97b4bbd8b33702094284542</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To know where are more unmarried females living in Hong Kong!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hong Kong Cycling Information Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A simple information map showing cycling track network in Hong Kong.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://arcg.is/1uGqC40</t>
+  </si>
+  <si>
+    <t>Low-altitude current situation dashboard (with Terrain) 3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A dashboard that shows how open data from HKGOVT and drone live routes (just demo) for quick decision making.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/e9226848248a47788ff5f5f1e3f5920f/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Smart and Green Mass Transit System in East Kowloon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The route of new railway from georeferenced General Layout Plans.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/953175648ca149bbb159963c607d2620/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cycling Track Coverage in Hong Kong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p4.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p5.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -119,7 +194,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -128,6 +203,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -464,46 +542,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35B43E3-CBE3-1E4D-8272-02E2CB7B0D41}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="49.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52" style="3" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" ht="34">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="68">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CC2950EF-E78D-AB4C-9C70-B5BB9CCD649C}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{287C1C6D-29E1-554B-B197-1AD4A11D3590}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{CA7223C9-C62E-A344-8836-B78E1FBD048E}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{C118AFF8-A7BF-604C-A83C-2FA47D744088}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{D370A6D7-2DA7-1143-9FAE-DEE2EAC3E5EC}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{A0BA9A6E-334B-7B41-AF49-A4FEBE79E579}"/>
+    <hyperlink ref="A3:A6" r:id="rId6" display="https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/p1.png" xr:uid="{847EC512-5D57-3048-B667-726A6C170082}"/>
+    <hyperlink ref="A3" r:id="rId7" xr:uid="{B260830E-70C4-7146-ADCB-6C55DBD9E2C2}"/>
+    <hyperlink ref="A4" r:id="rId8" xr:uid="{BB2D306D-72DE-DF4C-A2EA-000BF90D96DD}"/>
+    <hyperlink ref="A5" r:id="rId9" xr:uid="{6910317B-9691-444C-9967-7CE7E06E65F1}"/>
+    <hyperlink ref="A6" r:id="rId10" xr:uid="{ACC74FC1-3E8B-3C43-A5E4-FF7288EC6BE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>